<commit_message>
Added scripts for reports date coverage
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micadeguzman/eclipse-workspace/CTXBillingPortal/src/test/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CTXBillingPortal\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACF98A0-9D26-A24D-99FA-508ED7C3514C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="2" r:id="rId1"/>
-    <sheet name="SearchRep" sheetId="4" r:id="rId2"/>
-    <sheet name="Login" sheetId="3" r:id="rId3"/>
+    <sheet name="Reports" sheetId="5" r:id="rId2"/>
+    <sheet name="SearchRep" sheetId="4" r:id="rId3"/>
+    <sheet name="Login" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>TCID</t>
   </si>
@@ -90,15 +90,61 @@
   </si>
   <si>
     <t>Search_Reports</t>
+  </si>
+  <si>
+    <t>Daily Reports</t>
+  </si>
+  <si>
+    <t>Export_Daily_Report</t>
+  </si>
+  <si>
+    <t>02/27/2021</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Yearly</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>02/2/2021</t>
+  </si>
+  <si>
+    <t>04/27/2021</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>01/27/2020</t>
+  </si>
+  <si>
+    <t>JUNE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -113,7 +159,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -128,7 +175,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -136,15 +183,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -459,19 +558,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -487,15 +586,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -503,67 +602,83 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
         <v>1</v>
       </c>
     </row>
@@ -573,21 +688,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9BEE02-1E11-FD44-84A6-576240E01540}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.9140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.08203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.58203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.9140625" customWidth="1"/>
+    <col min="8" max="8" width="14.9140625" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -597,44 +782,51 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added script for reports date coverage
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>TCID</t>
   </si>
@@ -122,13 +122,16 @@
     <t>04/27/2021</t>
   </si>
   <si>
-    <t>2020</t>
-  </si>
-  <si>
     <t>01/27/2020</t>
   </si>
   <si>
-    <t>JUNE</t>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>MAY</t>
   </si>
 </sst>
 </file>
@@ -561,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -691,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -722,13 +725,13 @@
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>29</v>
@@ -736,7 +739,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>30</v>
@@ -751,9 +754,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="C2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
minor updates on reports
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CTXBillingPortal\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micadeguzman/eclipse-workspace/CTXBillingPortal/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D9E091-07E4-8047-BEE9-BEDC62CB06F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="2" r:id="rId1"/>
@@ -95,9 +96,6 @@
     <t>Daily Reports</t>
   </si>
   <si>
-    <t>Export_Daily_Report</t>
-  </si>
-  <si>
     <t>02/27/2021</t>
   </si>
   <si>
@@ -131,13 +129,16 @@
     <t>2021</t>
   </si>
   <si>
-    <t>MAY</t>
+    <t>Export_Daily_Reports</t>
+  </si>
+  <si>
+    <t>JANUARY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -561,19 +562,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -589,7 +590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -597,7 +598,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -605,15 +606,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -621,23 +622,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -645,7 +646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -653,7 +654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -661,7 +662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -669,7 +670,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -677,12 +678,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -691,64 +692,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.9140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.08203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.58203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14.9140625" customWidth="1"/>
-    <col min="8" max="8" width="14.9140625" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D7" s="7"/>
     </row>
   </sheetData>
@@ -758,21 +759,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -783,20 +784,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -807,7 +808,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -815,18 +816,18 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added alert handling & script optimization
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micadeguzman/eclipse-workspace/CTXBillingPortal/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D9E091-07E4-8047-BEE9-BEDC62CB06F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A35421-A80D-5E4D-985D-126B094941EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>TCID</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Logout_LogoutOption</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>ResetPassword_viaForgotPassword</t>
   </si>
   <si>
@@ -114,25 +111,22 @@
     <t>Base</t>
   </si>
   <si>
-    <t>02/2/2021</t>
-  </si>
-  <si>
-    <t>04/27/2021</t>
-  </si>
-  <si>
-    <t>01/27/2020</t>
-  </si>
-  <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
     <t>Export_Daily_Reports</t>
   </si>
   <si>
     <t>JANUARY</t>
+  </si>
+  <si>
+    <t>01/01/2021</t>
+  </si>
+  <si>
+    <t>01/01/2020</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>View_Profile</t>
   </si>
 </sst>
 </file>
@@ -563,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,7 +589,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -608,10 +602,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -627,7 +621,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -635,15 +629,15 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -651,7 +645,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -659,31 +653,39 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -696,7 +698,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,16 +714,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -729,18 +731,18 @@
         <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>29</v>
@@ -770,12 +772,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -805,7 +807,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -816,7 +818,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
modified testcases package and revised scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micadeguzman/eclipse-workspace/CTXBillingPortal/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BFE327-747B-4D47-B140-AE79AB88FAFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D870C54A-B572-2043-A44A-DAF80C15F427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>TCID</t>
   </si>
@@ -129,7 +129,16 @@
     <t>View_Profile</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Filter_Daily_Reports</t>
+  </si>
+  <si>
+    <t>Filter_Monthly_Reports</t>
+  </si>
+  <si>
+    <t>Filter_Yearly_Reports</t>
+  </si>
+  <si>
+    <t>Filter_Custom_Reports</t>
   </si>
 </sst>
 </file>
@@ -560,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,7 +614,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -613,7 +622,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -621,7 +630,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -629,7 +638,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -637,7 +646,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -645,7 +654,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -653,15 +662,15 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -669,7 +678,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -677,7 +686,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -685,9 +694,41 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B19" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified TestActions and TestBase class to align with updated site
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micadeguzman/eclipse-workspace/CTXBillingPortal/src/test/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micadeguzman/eclipse-workspace/ctxbillingportal_gitlab/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D870C54A-B572-2043-A44A-DAF80C15F427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EF6A97-3077-B74B-95C6-383701ED87CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>TCID</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Filter_Custom_Reports</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -572,7 +575,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -721,7 +724,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>